<commit_message>
Several modification, cpu part should work fine
</commit_message>
<xml_diff>
--- a/Project work/Runtime stat.xlsx
+++ b/Project work/Runtime stat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\own\github\Parallel-Dev-2025\Project work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\parallel dev (XPGMCH)\Parallel-Dev-2025\Project work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EBEFD6-26A8-4E65-8EE3-33840213079A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC591E05-1B9B-43B1-BE97-970AC9D1F763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="1" r:id="rId1"/>
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
         <v>100000</v>
       </c>
       <c r="C3">
-        <v>1000</v>
+        <v>32000</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
@@ -443,18 +443,18 @@
         <v>100000</v>
       </c>
       <c r="H3">
-        <v>1000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="C4">
         <v>32000</v>
       </c>
       <c r="G4">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="H4">
         <v>32000</v>
@@ -474,33 +474,19 @@
         <v>32000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B6">
-        <v>100000</v>
-      </c>
-      <c r="C6">
-        <v>1000</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>100000</v>
-      </c>
-      <c r="H6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>100000</v>
       </c>
       <c r="C7">
         <v>32000</v>
       </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
       <c r="G7">
         <v>100000</v>
       </c>
@@ -509,13 +495,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
+      <c r="B8">
         <v>1000000</v>
       </c>
       <c r="C8">
         <v>32000</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8">
         <v>1000000</v>
       </c>
       <c r="H8">
@@ -524,13 +510,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="C9">
         <v>32000</v>
       </c>
       <c r="G9" s="1">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="H9">
         <v>32000</v>
@@ -538,45 +524,45 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="C10">
+        <v>32000</v>
+      </c>
+      <c r="G10" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="H10">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
         <v>100000000</v>
       </c>
-      <c r="C10">
-        <v>32000</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="C11">
+        <v>32000</v>
+      </c>
+      <c r="G11" s="1">
         <v>100000000</v>
       </c>
-      <c r="H10">
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="H11">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B12">
-        <v>100000</v>
-      </c>
-      <c r="C12">
-        <v>1000</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12">
-        <v>100000</v>
-      </c>
-      <c r="H12">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>100000</v>
       </c>
       <c r="C13">
         <v>32000</v>
       </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
       <c r="G13">
         <v>100000</v>
       </c>
@@ -585,13 +571,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
+      <c r="B14">
         <v>1000000</v>
       </c>
       <c r="C14">
         <v>32000</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14">
         <v>1000000</v>
       </c>
       <c r="H14">
@@ -600,13 +586,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="C15">
         <v>32000</v>
       </c>
       <c r="G15" s="1">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="H15">
         <v>32000</v>
@@ -614,15 +600,29 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="C16">
+        <v>32000</v>
+      </c>
+      <c r="G16" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="H16">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <v>100000000</v>
       </c>
-      <c r="C16">
-        <v>32000</v>
-      </c>
-      <c r="G16" s="1">
+      <c r="C17">
+        <v>32000</v>
+      </c>
+      <c r="G17" s="1">
         <v>100000000</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>32000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working is going on
</commit_message>
<xml_diff>
--- a/Project work/Runtime stat.xlsx
+++ b/Project work/Runtime stat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\parallel dev (XPGMCH)\Parallel-Dev-2025\Project work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\own\github\Parallel-Dev-2025\Project work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC591E05-1B9B-43B1-BE97-970AC9D1F763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EBEFD6-26A8-4E65-8EE3-33840213079A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Doc" sheetId="1" r:id="rId1"/>
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
         <v>100000</v>
       </c>
       <c r="C3">
-        <v>32000</v>
+        <v>1000</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
@@ -443,18 +443,18 @@
         <v>100000</v>
       </c>
       <c r="H3">
-        <v>32000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="C4">
         <v>32000</v>
       </c>
       <c r="G4">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="H4">
         <v>32000</v>
@@ -474,19 +474,33 @@
         <v>32000</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>100000</v>
+      </c>
+      <c r="C6">
+        <v>1000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>100000</v>
+      </c>
+      <c r="H6">
+        <v>1000</v>
+      </c>
+    </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
       <c r="B7">
         <v>100000</v>
       </c>
       <c r="C7">
         <v>32000</v>
       </c>
-      <c r="F7" t="s">
-        <v>1</v>
-      </c>
       <c r="G7">
         <v>100000</v>
       </c>
@@ -495,13 +509,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="B8" s="1">
         <v>1000000</v>
       </c>
       <c r="C8">
         <v>32000</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>1000000</v>
       </c>
       <c r="H8">
@@ -510,13 +524,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="C9">
         <v>32000</v>
       </c>
       <c r="G9" s="1">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="H9">
         <v>32000</v>
@@ -524,45 +538,45 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
-        <v>10000000</v>
+        <v>100000000</v>
       </c>
       <c r="C10">
         <v>32000</v>
       </c>
       <c r="G10" s="1">
-        <v>10000000</v>
+        <v>100000000</v>
       </c>
       <c r="H10">
         <v>32000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="C11">
-        <v>32000</v>
-      </c>
-      <c r="G11" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="H11">
-        <v>32000</v>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>100000</v>
+      </c>
+      <c r="C12">
+        <v>1000</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>100000</v>
+      </c>
+      <c r="H12">
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
       <c r="B13">
         <v>100000</v>
       </c>
       <c r="C13">
         <v>32000</v>
       </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
       <c r="G13">
         <v>100000</v>
       </c>
@@ -571,13 +585,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="B14" s="1">
         <v>1000000</v>
       </c>
       <c r="C14">
         <v>32000</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>1000000</v>
       </c>
       <c r="H14">
@@ -586,13 +600,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="C15">
         <v>32000</v>
       </c>
       <c r="G15" s="1">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="H15">
         <v>32000</v>
@@ -600,29 +614,15 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
-        <v>10000000</v>
+        <v>100000000</v>
       </c>
       <c r="C16">
         <v>32000</v>
       </c>
       <c r="G16" s="1">
-        <v>10000000</v>
+        <v>100000000</v>
       </c>
       <c r="H16">
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="C17">
-        <v>32000</v>
-      </c>
-      <c r="G17" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="H17">
         <v>32000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final version, and datas
</commit_message>
<xml_diff>
--- a/Project work/Runtime stat.xlsx
+++ b/Project work/Runtime stat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\own\github\Parallel-Dev-2025\Project work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EBEFD6-26A8-4E65-8EE3-33840213079A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F099E0D-6261-40F6-8D37-08779FA0F54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>Without parallel code:</t>
   </si>
@@ -49,6 +49,117 @@
   </si>
   <si>
     <t>With parallel code:</t>
+  </si>
+  <si>
+    <t>Group size:</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>5.86</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>1.038</t>
+  </si>
+  <si>
+    <t>0.142</t>
+  </si>
+  <si>
+    <t>5.913</t>
+  </si>
+  <si>
+    <t>0.286</t>
+  </si>
+  <si>
+    <t>5.71</t>
+  </si>
+  <si>
+    <t>0.00058</t>
+  </si>
+  <si>
+    <t>1.272</t>
+  </si>
+  <si>
+    <t>0.087</t>
+  </si>
+  <si>
+    <t>7.842</t>
+  </si>
+  <si>
+    <t>1070.928</t>
+  </si>
+  <si>
+    <t>2610.193</t>
+  </si>
+  <si>
+    <t>0.191</t>
+  </si>
+  <si>
+    <t>4.654</t>
+  </si>
+  <si>
+    <t>1831.657</t>
+  </si>
+  <si>
+    <t>3141.782</t>
+  </si>
+  <si>
+    <t>0.2221</t>
+  </si>
+  <si>
+    <t>6.1200</t>
+  </si>
+  <si>
+    <t>20451.674</t>
+  </si>
+  <si>
+    <t>32.2300</t>
+  </si>
+  <si>
+    <t>33.94</t>
+  </si>
+  <si>
+    <t>26312.458</t>
+  </si>
+  <si>
+    <t>28870.271</t>
+  </si>
+  <si>
+    <t>30412.4</t>
+  </si>
+  <si>
+    <t>0.112</t>
+  </si>
+  <si>
+    <t>0.122</t>
+  </si>
+  <si>
+    <t>0.192</t>
+  </si>
+  <si>
+    <t>0.21</t>
+  </si>
+  <si>
+    <t>3.762</t>
+  </si>
+  <si>
+    <t>4.012</t>
+  </si>
+  <si>
+    <t>21.67</t>
+  </si>
+  <si>
+    <t>30.452</t>
+  </si>
+  <si>
+    <t>45.645</t>
+  </si>
+  <si>
+    <t>42.023</t>
   </si>
 </sst>
 </file>
@@ -90,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -98,6 +209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -378,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,33 +543,48 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="C3">
-        <v>1000</v>
+        <v>15000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="H3">
-        <v>1000</v>
+        <v>15000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="C4">
         <v>32000</v>
       </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
       <c r="G4">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="H4">
         <v>32000</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -465,165 +592,334 @@
         <v>1000000</v>
       </c>
       <c r="C5">
-        <v>32000</v>
+        <v>15000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
       </c>
       <c r="G5" s="1">
         <v>1000000</v>
       </c>
       <c r="H5">
-        <v>32000</v>
+        <v>15000</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>100000</v>
+      <c r="B6" s="1">
+        <v>1000000</v>
       </c>
       <c r="C6">
-        <v>1000</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>100000</v>
+        <v>32000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1000000</v>
       </c>
       <c r="H6">
-        <v>1000</v>
+        <v>32000</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>100000</v>
+      <c r="B7" s="1">
+        <v>100000000</v>
       </c>
       <c r="C7">
-        <v>32000</v>
-      </c>
-      <c r="G7">
-        <v>100000</v>
+        <v>15000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1">
+        <v>100000000</v>
       </c>
       <c r="H7">
-        <v>32000</v>
+        <v>15000</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
-        <v>1000000</v>
+        <v>100000000</v>
       </c>
       <c r="C8">
         <v>32000</v>
       </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
       <c r="G8" s="1">
-        <v>1000000</v>
+        <v>100000000</v>
       </c>
       <c r="H8">
         <v>32000</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <v>10000000</v>
-      </c>
-      <c r="C9">
-        <v>32000</v>
-      </c>
-      <c r="G9" s="1">
-        <v>10000000</v>
-      </c>
-      <c r="H9">
-        <v>32000</v>
+      <c r="I8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
-        <v>100000000</v>
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>10000</v>
       </c>
       <c r="C10">
-        <v>32000</v>
-      </c>
-      <c r="G10" s="1">
-        <v>100000000</v>
+        <v>15000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>10000</v>
       </c>
       <c r="H10">
-        <v>32000</v>
+        <v>15000</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>10000</v>
+      </c>
+      <c r="C11">
+        <v>32000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11">
+        <v>10000</v>
+      </c>
+      <c r="H11">
+        <v>32000</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>100000</v>
+      <c r="B12" s="1">
+        <v>1000000</v>
       </c>
       <c r="C12">
-        <v>1000</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12">
-        <v>100000</v>
+        <v>15000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1000000</v>
       </c>
       <c r="H12">
-        <v>1000</v>
+        <v>15000</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>100000</v>
+      <c r="B13" s="1">
+        <v>1000000</v>
       </c>
       <c r="C13">
         <v>32000</v>
       </c>
-      <c r="G13">
-        <v>100000</v>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1000000</v>
       </c>
       <c r="H13">
         <v>32000</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
-        <v>1000000</v>
+        <v>100000000</v>
       </c>
       <c r="C14">
-        <v>32000</v>
+        <v>15000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
       </c>
       <c r="G14" s="1">
-        <v>1000000</v>
+        <v>100000000</v>
       </c>
       <c r="H14">
-        <v>32000</v>
+        <v>15000</v>
+      </c>
+      <c r="I14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
-        <v>10000000</v>
+        <v>100000000</v>
       </c>
       <c r="C15">
         <v>32000</v>
       </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
       <c r="G15" s="1">
-        <v>10000000</v>
+        <v>100000000</v>
       </c>
       <c r="H15">
         <v>32000</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="C16">
-        <v>32000</v>
-      </c>
-      <c r="G16" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="H16">
-        <v>32000</v>
+      <c r="I15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>10000</v>
+      </c>
+      <c r="C17">
+        <v>15000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>10000</v>
+      </c>
+      <c r="H17">
+        <v>15000</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>10000</v>
+      </c>
+      <c r="C18">
+        <v>32000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18">
+        <v>10000</v>
+      </c>
+      <c r="H18">
+        <v>32000</v>
+      </c>
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C19">
+        <v>15000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="H19">
+        <v>15000</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C20">
+        <v>32000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="H20">
+        <v>32000</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="C21">
+        <v>15000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="H21">
+        <v>15000</v>
+      </c>
+      <c r="I21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="C22">
+        <v>32000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="H22">
+        <v>32000</v>
+      </c>
+      <c r="I22" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>